<commit_message>
refactor function's code; add an overall dataset, where each of its rows is the summary/overall_means row of all the other datasets
</commit_message>
<xml_diff>
--- a/analyzed-cell-data/all_image_set_data.xlsx
+++ b/analyzed-cell-data/all_image_set_data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSet_1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSet_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverallData" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,291 +436,276 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label_id</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>label_id</t>
+          <t>nucleus_mean_int</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>nucleus_mask_mean</t>
+          <t>nucleus_max_int</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>nucleus_mask_max</t>
+          <t>nucleus_area</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>nucleus_mask_area</t>
+          <t>inner_donut_mean_int</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>donut_mask_mean</t>
+          <t>inner_donut_max_int</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>donut_mask_max</t>
+          <t>inner_donut_area</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>donut_mask_area</t>
+          <t>outer_donut_mean_int</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>outer_donut_mask_mean</t>
+          <t>outer_donut_max_int</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>outer_donut_mask_max</t>
+          <t>outer_donut_area</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>outer_donut_mask_area</t>
+          <t>regional_mean_int</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>regional_mask_mean</t>
+          <t>regional_max_int</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>regional_mask_max</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>regional_mask_area</t>
+          <t>regional_area</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="n">
+        <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>0.1626114701791704</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1626114701791704</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>48.02252142732571</v>
       </c>
       <c r="E2" t="n">
-        <v>48.02252142732571</v>
+        <v>0.1440184780698451</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1440184780698451</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>33.25136646255208</v>
       </c>
       <c r="H2" t="n">
-        <v>33.25136646255208</v>
+        <v>0.07209653092006033</v>
       </c>
       <c r="I2" t="n">
-        <v>0.07209653092006033</v>
+        <v>0.2470588235294118</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2470588235294118</v>
+        <v>3.416236280399187</v>
       </c>
       <c r="K2" t="n">
-        <v>3.416236280399187</v>
+        <v>0.1506818159046961</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1506818159046961</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
         <v>84.69012417027697</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="n">
+        <v>31</v>
       </c>
       <c r="B3" t="n">
-        <v>31</v>
+        <v>0.1119720437194486</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1119720437194486</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>58.82433519011171</v>
       </c>
       <c r="E3" t="n">
-        <v>58.82433519011171</v>
+        <v>0.1366438417713556</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1366438417713556</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>47.04645391864023</v>
       </c>
       <c r="H3" t="n">
-        <v>47.04645391864023</v>
+        <v>0.07705714764538293</v>
       </c>
       <c r="I3" t="n">
-        <v>0.07705714764538293</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3333333333333333</v>
+        <v>6.149225304718536</v>
       </c>
       <c r="K3" t="n">
-        <v>6.149225304718536</v>
+        <v>0.1196875261516743</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1196875261516743</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
         <v>112.0200144134705</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="n">
+        <v>37</v>
       </c>
       <c r="B4" t="n">
-        <v>37</v>
+        <v>0.1119702513454273</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1119702513454273</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="D4" t="n">
+        <v>47.56702325660582</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1079381207984508</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8941176470588236</v>
+      </c>
+      <c r="G4" t="n">
+        <v>55.50570566058106</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.07918767507002801</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.396078431372549</v>
+      </c>
+      <c r="J4" t="n">
+        <v>10.41138675931181</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.1067011810156877</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="E4" t="n">
-        <v>47.56702325660582</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.1079381207984508</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="M4" t="n">
+        <v>113.4841156764987</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>48</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1093395252837977</v>
+      </c>
+      <c r="C5" t="n">
         <v>0.8941176470588236</v>
       </c>
-      <c r="H4" t="n">
-        <v>55.50570566058106</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.07918767507002801</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.396078431372549</v>
-      </c>
-      <c r="K4" t="n">
-        <v>10.41138675931181</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.1067011810156877</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.9411764705882353</v>
-      </c>
-      <c r="N4" t="n">
-        <v>113.4841156764987</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>48</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.1093395252837977</v>
-      </c>
       <c r="D5" t="n">
-        <v>0.8941176470588236</v>
+        <v>59.3449045280773</v>
       </c>
       <c r="E5" t="n">
-        <v>59.3449045280773</v>
+        <v>0.1424467815678277</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1424467815678277</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>65.39652308192728</v>
       </c>
       <c r="H5" t="n">
-        <v>65.39652308192728</v>
+        <v>0.09470805754948572</v>
       </c>
       <c r="I5" t="n">
-        <v>0.09470805754948572</v>
+        <v>0.7647058823529411</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7647058823529411</v>
+        <v>12.72141319653411</v>
       </c>
       <c r="K5" t="n">
-        <v>12.72141319653411</v>
+        <v>0.1229858790753571</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1229858790753571</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" t="n">
         <v>137.4628408065387</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>overall_means</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>0.123973322631961</v>
+      </c>
       <c r="C6" t="n">
-        <v>0.123973322631961</v>
+        <v>0.9588235294117647</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9588235294117647</v>
+        <v>53.43969610053013</v>
       </c>
       <c r="E6" t="n">
-        <v>53.43969610053013</v>
+        <v>0.1327618055518698</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1327618055518698</v>
+        <v>0.9735294117647059</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9735294117647059</v>
+        <v>50.30001228092517</v>
       </c>
       <c r="H6" t="n">
-        <v>50.30001228092517</v>
+        <v>0.08076235279623925</v>
       </c>
       <c r="I6" t="n">
-        <v>0.08076235279623925</v>
+        <v>0.4352941176470588</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4352941176470588</v>
+        <v>8.174565385240911</v>
       </c>
       <c r="K6" t="n">
-        <v>8.174565385240911</v>
+        <v>0.1250141005368538</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1250141005368538</v>
+        <v>0.9852941176470589</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9852941176470589</v>
-      </c>
-      <c r="N6" t="n">
         <v>111.9142737666962</v>
       </c>
     </row>
@@ -734,7 +720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,379 +729,530 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label_id</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>label_id</t>
+          <t>nucleus_mean_int</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>nucleus_mask_mean</t>
+          <t>nucleus_max_int</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>nucleus_mask_max</t>
+          <t>nucleus_area</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>nucleus_mask_area</t>
+          <t>inner_donut_mean_int</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>donut_mask_mean</t>
+          <t>inner_donut_max_int</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>donut_mask_max</t>
+          <t>inner_donut_area</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>donut_mask_area</t>
+          <t>outer_donut_mean_int</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>outer_donut_mask_mean</t>
+          <t>outer_donut_max_int</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>outer_donut_mask_max</t>
+          <t>outer_donut_area</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>outer_donut_mask_area</t>
+          <t>regional_mean_int</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>regional_mask_mean</t>
+          <t>regional_max_int</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>regional_mask_max</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>regional_mask_area</t>
+          <t>regional_area</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="n">
+        <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>0.1360995506967306</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1360995506967306</v>
+        <v>0.9803921568627451</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9803921568627451</v>
+        <v>43.4024685528811</v>
       </c>
       <c r="E2" t="n">
-        <v>43.4024685528811</v>
+        <v>0.1899224429656255</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1899224429656255</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>86.21929660055089</v>
       </c>
       <c r="H2" t="n">
-        <v>86.21929660055089</v>
+        <v>0.1500326797385621</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1500326797385621</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>17.76442865807577</v>
       </c>
       <c r="K2" t="n">
-        <v>17.76442865807577</v>
+        <v>0.1686490082133057</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1686490082133057</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
         <v>147.3861938115078</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="n">
+        <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>0.1215669961828325</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1215669961828325</v>
+        <v>0.8470588235294118</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8470588235294118</v>
+        <v>53.00046572162167</v>
       </c>
       <c r="E3" t="n">
-        <v>53.00046572162167</v>
+        <v>0.2324628796109472</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2324628796109472</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>70.79742996332028</v>
       </c>
       <c r="H3" t="n">
-        <v>70.79742996332028</v>
+        <v>0.2638641680534452</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2638641680534452</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>18.15485566154996</v>
       </c>
       <c r="K3" t="n">
-        <v>18.15485566154996</v>
+        <v>0.1938863943721191</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1938863943721191</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
         <v>141.9527513464919</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="n">
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>0.1378433327468574</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1378433327468574</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>44.76896306504077</v>
       </c>
       <c r="E4" t="n">
-        <v>44.76896306504077</v>
+        <v>0.2100929707185681</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2100929707185681</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>80.65571180104365</v>
       </c>
       <c r="H4" t="n">
-        <v>80.65571180104365</v>
+        <v>0.09118994162550514</v>
       </c>
       <c r="I4" t="n">
-        <v>0.09118994162550514</v>
+        <v>0.5450980392156862</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5450980392156862</v>
+        <v>13.33958928536825</v>
       </c>
       <c r="K4" t="n">
-        <v>13.33958928536825</v>
+        <v>0.1732398020405648</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1732398020405648</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" t="n">
         <v>138.7642641514527</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="n">
+        <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>0.100323258063755</v>
       </c>
       <c r="C5" t="n">
-        <v>0.100323258063755</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>51.08086628787355</v>
       </c>
       <c r="E5" t="n">
-        <v>51.08086628787355</v>
+        <v>0.2117423543940232</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2117423543940232</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>81.4691013916149</v>
       </c>
       <c r="H5" t="n">
-        <v>81.4691013916149</v>
+        <v>0.126703146374829</v>
       </c>
       <c r="I5" t="n">
-        <v>0.126703146374829</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>18.21992682879566</v>
       </c>
       <c r="K5" t="n">
-        <v>18.21992682879566</v>
+        <v>0.160605437161749</v>
       </c>
       <c r="L5" t="n">
-        <v>0.160605437161749</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" t="n">
         <v>150.7698945082841</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="n">
+        <v>33</v>
       </c>
       <c r="B6" t="n">
-        <v>33</v>
+        <v>0.1551651695160823</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1551651695160823</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>34.42264747297466</v>
       </c>
       <c r="E6" t="n">
-        <v>34.42264747297466</v>
+        <v>0.2011040193203381</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2011040193203381</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>61.58985979805391</v>
       </c>
       <c r="H6" t="n">
-        <v>61.58985979805391</v>
+        <v>0.08856486567462299</v>
       </c>
       <c r="I6" t="n">
-        <v>0.08856486567462299</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5882352941176471</v>
+        <v>11.28984751712874</v>
       </c>
       <c r="K6" t="n">
-        <v>11.28984751712874</v>
+        <v>0.1725894972439492</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1725894972439492</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" t="n">
         <v>107.3023547881573</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="n">
+        <v>45</v>
       </c>
       <c r="B7" t="n">
-        <v>45</v>
+        <v>0.1086060090552262</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1086060090552262</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>46.00531524270905</v>
       </c>
       <c r="E7" t="n">
-        <v>46.00531524270905</v>
+        <v>0.2266368760994902</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2266368760994902</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>71.48067721940012</v>
       </c>
       <c r="H7" t="n">
-        <v>71.48067721940012</v>
+        <v>0.1221884498480243</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1221884498480243</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>13.66494512159675</v>
       </c>
       <c r="K7" t="n">
-        <v>13.66494512159675</v>
+        <v>0.1709525936957061</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1709525936957061</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
         <v>131.1509375837059</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>overall_means</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>0.126600719376914</v>
+      </c>
       <c r="C8" t="n">
+        <v>0.9712418300653595</v>
+      </c>
+      <c r="D8" t="n">
+        <v>45.44678772385013</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2119935905181654</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>75.36867946233063</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1404238752191648</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.8555555555555555</v>
+      </c>
+      <c r="J8" t="n">
+        <v>15.40559884541919</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.1733204554545656</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>136.2210660315999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>image_set</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nucleus_mean_int</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nucleus_max_int</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>nucleus_area</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>inner_donut_mean_int</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>inner_donut_max_int</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>inner_donut_area</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>outer_donut_mean_int</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>outer_donut_max_int</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>outer_donut_area</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>regional_mean_int</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>regional_max_int</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>regional_area</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ImageSet_1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.123973322631961</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9588235294117647</v>
+      </c>
+      <c r="D2" t="n">
+        <v>53.43969610053013</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1327618055518698</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9735294117647059</v>
+      </c>
+      <c r="G2" t="n">
+        <v>50.30001228092517</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.08076235279623925</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.4352941176470588</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8.174565385240911</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.1250141005368538</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.9852941176470589</v>
+      </c>
+      <c r="M2" t="n">
+        <v>111.9142737666962</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ImageSet_2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>0.126600719376914</v>
       </c>
-      <c r="D8" t="n">
+      <c r="C3" t="n">
         <v>0.9712418300653595</v>
       </c>
-      <c r="E8" t="n">
+      <c r="D3" t="n">
         <v>45.44678772385013</v>
       </c>
-      <c r="F8" t="n">
+      <c r="E3" t="n">
         <v>0.2119935905181654</v>
       </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
         <v>75.36867946233063</v>
       </c>
-      <c r="I8" t="n">
+      <c r="H3" t="n">
         <v>0.1404238752191648</v>
       </c>
-      <c r="J8" t="n">
+      <c r="I3" t="n">
         <v>0.8555555555555555</v>
       </c>
-      <c r="K8" t="n">
+      <c r="J3" t="n">
         <v>15.40559884541919</v>
       </c>
-      <c r="L8" t="n">
+      <c r="K3" t="n">
         <v>0.1733204554545656</v>
       </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" t="n">
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
         <v>136.2210660315999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add iteration through multiple folders with all microscopy planes; add customization to allow user to choose which planes they want to use for analysis; add logic such that p115 analysis occurs for 3 different planes: 1 below the nucleus plane, 1 at the nucleus plane, and 1 above the nucleus plane
</commit_message>
<xml_diff>
--- a/analyzed-cell-data/all_image_set_data.xlsx
+++ b/analyzed-cell-data/all_image_set_data.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSet_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSet_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverallData" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverallData" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,210 +502,175 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>29</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>42z1</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1626114701791704</v>
+        <v>0.06594974973982853</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="D2" t="n">
-        <v>48.02252142732571</v>
+        <v>19.5430376658214</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1440184780698451</v>
+        <v>0.05776870401088852</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.3176470588235294</v>
       </c>
       <c r="G2" t="n">
-        <v>33.25136646255208</v>
+        <v>13.98765640041024</v>
       </c>
       <c r="H2" t="n">
-        <v>0.07209653092006033</v>
+        <v>0.0553606237816764</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2470588235294118</v>
+        <v>0.207843137254902</v>
       </c>
       <c r="J2" t="n">
-        <v>3.416236280399187</v>
+        <v>2.347809939548764</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1506818159046961</v>
+        <v>0.06184726522187822</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="M2" t="n">
-        <v>84.69012417027697</v>
+        <v>35.8785040057804</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>31</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>42z2</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1119720437194486</v>
+        <v>0.06594974973982853</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="D3" t="n">
-        <v>58.82433519011171</v>
+        <v>19.5430376658214</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1366438417713556</v>
+        <v>0.05776870401088852</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0.3176470588235294</v>
       </c>
       <c r="G3" t="n">
-        <v>47.04645391864023</v>
+        <v>13.98765640041024</v>
       </c>
       <c r="H3" t="n">
-        <v>0.07705714764538293</v>
+        <v>0.0553606237816764</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.207843137254902</v>
       </c>
       <c r="J3" t="n">
-        <v>6.149225304718536</v>
+        <v>2.347809939548764</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1196875261516743</v>
+        <v>0.06184726522187822</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="M3" t="n">
-        <v>112.0200144134705</v>
+        <v>35.8785040057804</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>37</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>42z3</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1119702513454273</v>
+        <v>0.06594974973982853</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="D4" t="n">
-        <v>47.56702325660582</v>
+        <v>19.5430376658214</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1079381207984508</v>
+        <v>0.05776870401088852</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8941176470588236</v>
+        <v>0.3176470588235294</v>
       </c>
       <c r="G4" t="n">
-        <v>55.50570566058106</v>
+        <v>13.98765640041024</v>
       </c>
       <c r="H4" t="n">
-        <v>0.07918767507002801</v>
+        <v>0.0553606237816764</v>
       </c>
       <c r="I4" t="n">
-        <v>0.396078431372549</v>
+        <v>0.207843137254902</v>
       </c>
       <c r="J4" t="n">
-        <v>10.41138675931181</v>
+        <v>2.347809939548764</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1067011810156877</v>
+        <v>0.06184726522187822</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="M4" t="n">
-        <v>113.4841156764987</v>
+        <v>35.8785040057804</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>48</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>overall_means</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1093395252837977</v>
+        <v>0.06594974973982853</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8941176470588236</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="D5" t="n">
-        <v>59.3449045280773</v>
+        <v>19.5430376658214</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1424467815678277</v>
+        <v>0.05776870401088852</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0.3176470588235294</v>
       </c>
       <c r="G5" t="n">
-        <v>65.39652308192728</v>
+        <v>13.98765640041024</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09470805754948572</v>
+        <v>0.05536062378167641</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7647058823529411</v>
+        <v>0.207843137254902</v>
       </c>
       <c r="J5" t="n">
-        <v>12.72141319653411</v>
+        <v>2.347809939548764</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1229858790753571</v>
+        <v>0.06184726522187822</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="M5" t="n">
-        <v>137.4628408065387</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>overall_means</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.123973322631961</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.9588235294117647</v>
-      </c>
-      <c r="D6" t="n">
-        <v>53.43969610053013</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.1327618055518698</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.9735294117647059</v>
-      </c>
-      <c r="G6" t="n">
-        <v>50.30001228092517</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.08076235279623925</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.4352941176470588</v>
-      </c>
-      <c r="J6" t="n">
-        <v>8.174565385240911</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.1250141005368538</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.9852941176470589</v>
-      </c>
-      <c r="M6" t="n">
-        <v>111.9142737666962</v>
+        <v>35.8785040057804</v>
       </c>
     </row>
   </sheetData>
@@ -720,7 +684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,381 +695,6 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>label_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>nucleus_mean_int</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>nucleus_max_int</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>nucleus_area</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>inner_donut_mean_int</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>inner_donut_max_int</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>inner_donut_area</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>outer_donut_mean_int</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>outer_donut_max_int</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>outer_donut_area</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>regional_mean_int</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>regional_max_int</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>regional_area</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.1360995506967306</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.9803921568627451</v>
-      </c>
-      <c r="D2" t="n">
-        <v>43.4024685528811</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.1899224429656255</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>86.21929660055089</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.1500326797385621</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>17.76442865807577</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.1686490082133057</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>147.3861938115078</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.1215669961828325</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.8470588235294118</v>
-      </c>
-      <c r="D3" t="n">
-        <v>53.00046572162167</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.2324628796109472</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>70.79742996332028</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2638641680534452</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>18.15485566154996</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.1938863943721191</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>141.9527513464919</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.1378433327468574</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>44.76896306504077</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.2100929707185681</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>80.65571180104365</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.09118994162550514</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.5450980392156862</v>
-      </c>
-      <c r="J4" t="n">
-        <v>13.33958928536825</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1732398020405648</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>138.7642641514527</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>30</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.100323258063755</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>51.08086628787355</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2117423543940232</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>81.4691013916149</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.126703146374829</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>18.21992682879566</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.160605437161749</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>150.7698945082841</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>33</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.1551651695160823</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>34.42264747297466</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.2011040193203381</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>61.58985979805391</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.08856486567462299</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.5882352941176471</v>
-      </c>
-      <c r="J6" t="n">
-        <v>11.28984751712874</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.1725894972439492</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>107.3023547881573</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>45</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.1086060090552262</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>46.00531524270905</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.2266368760994902</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>71.48067721940012</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.1221884498480243</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>13.66494512159675</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.1709525936957061</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="n">
-        <v>131.1509375837059</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>overall_means</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.126600719376914</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.9712418300653595</v>
-      </c>
-      <c r="D8" t="n">
-        <v>45.44678772385013</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.2119935905181654</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>75.36867946233063</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.1404238752191648</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.8555555555555555</v>
-      </c>
-      <c r="J8" t="n">
-        <v>15.40559884541919</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.1733204554545656</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="n">
-        <v>136.2210660315999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
           <t>image_set</t>
         </is>
       </c>
@@ -1177,83 +766,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.123973322631961</v>
+        <v>0.06594974973982853</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9588235294117647</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="D2" t="n">
-        <v>53.43969610053013</v>
+        <v>19.5430376658214</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1327618055518698</v>
+        <v>0.05776870401088852</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9735294117647059</v>
+        <v>0.3176470588235294</v>
       </c>
       <c r="G2" t="n">
-        <v>50.30001228092517</v>
+        <v>13.98765640041024</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08076235279623925</v>
+        <v>0.05536062378167641</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4352941176470588</v>
+        <v>0.207843137254902</v>
       </c>
       <c r="J2" t="n">
-        <v>8.174565385240911</v>
+        <v>2.347809939548764</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1250141005368538</v>
+        <v>0.06184726522187822</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9852941176470589</v>
+        <v>0.4392156862745098</v>
       </c>
       <c r="M2" t="n">
-        <v>111.9142737666962</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ImageSet_2</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.126600719376914</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.9712418300653595</v>
-      </c>
-      <c r="D3" t="n">
-        <v>45.44678772385013</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.2119935905181654</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>75.36867946233063</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.1404238752191648</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.8555555555555555</v>
-      </c>
-      <c r="J3" t="n">
-        <v>15.40559884541919</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.1733204554545656</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>136.2210660315999</v>
+        <v>35.8785040057804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>